<commit_message>
F3.2 clean up & optimizations
</commit_message>
<xml_diff>
--- a/test/altsheet.xlsx
+++ b/test/altsheet.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
-  <si>
-    <t>floater.gif</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>C6030042_01.png</t>
   </si>
@@ -129,9 +126,6 @@
     <t>C6030043_35.jpg</t>
   </si>
   <si>
-    <t>join plenti for free. start earning points today! plenti is a new way to get rewards at macy's and lots of other places. terms and conditions apply.</t>
-  </si>
-  <si>
     <t>buy online, pick up in store and get extra 20% off your next store purchase! exclusions apply.</t>
   </si>
   <si>
@@ -228,23 +222,39 @@
     <t>GIVE A GIFT, GET A GIFT TAKE $20 OFF Your next purchase of $50 or more when you shop a couple’s registry.</t>
   </si>
   <si>
-    <t>Need Spring Style help? Let us find the perfect look or gift for every occasion — It’s fun, fast and free!</t>
-  </si>
-  <si>
     <t>Say hello to Plenti Start earning points today! Plenti is a great way to get rewards at Macy’s and lots of other places. Terms and conditions apply.</t>
   </si>
   <si>
     <t>ENJOY EXTRA SAVINGS IN STORES! get savings pass. get $10 off savings pass. SHOP THE CATALOG. find a store</t>
+  </si>
+  <si>
+    <t>Need Spring Style help? Let us find the perfect look or gift for every occasion. It is fun, fast and free!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,13 +277,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -603,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B36"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -619,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -627,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -659,7 +673,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -667,7 +681,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -675,7 +689,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -683,7 +697,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -691,7 +705,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -699,7 +713,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -707,7 +721,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -715,7 +729,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -723,7 +737,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -731,7 +745,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -739,7 +753,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -747,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -755,7 +769,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -763,7 +777,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -771,7 +785,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -779,7 +793,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -787,7 +801,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -795,7 +809,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -803,7 +817,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -811,7 +825,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -819,7 +833,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -827,7 +841,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -835,7 +849,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -843,7 +857,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -851,7 +865,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -859,7 +873,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -867,7 +881,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -875,7 +889,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -883,7 +897,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -891,19 +905,12 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>